<commit_message>
Did Changes in Organization Name
</commit_message>
<xml_diff>
--- a/Vtiger_Automation_Framework/src/test/resources/TestData/Vtigerdata.xlsx
+++ b/Vtiger_Automation_Framework/src/test/resources/TestData/Vtigerdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Keshav Sir Java\Oops Practice\Vtiger_Automation_Framework\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rutusmita prusty\git\repository4\Vtiger_Automation_Framework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DDF9E1-95DD-4648-81FA-90896CFEB16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E3204D-4A55-4B18-B45F-C1091F28ACE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2C08E847-41E6-4927-BBE6-948138CD3F06}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Microsoft</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Wipro</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324787E2-269B-4516-89F3-C80AFFED9520}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,6 +454,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>